<commit_message>
added some progress on owner parsing
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/xlsx/garages_report.xlsx
+++ b/src/main/resources/templates/xlsx/garages_report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t xml:space="preserve">Obec</t>
   </si>
@@ -49,7 +49,19 @@
     <t xml:space="preserve">Iné údaje</t>
   </si>
   <si>
-    <t xml:space="preserve">Vlastník</t>
+    <t xml:space="preserve">Dátum narodenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priezvisko a Meno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ulica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSČ</t>
   </si>
   <si>
     <t xml:space="preserve">Spoluvlastnícky podiel</t>
@@ -85,7 +97,19 @@
     <t xml:space="preserve">${row.ine_udaje}</t>
   </si>
   <si>
-    <t xml:space="preserve">${row.vlastnik}</t>
+    <t xml:space="preserve">${row.owner_birthDate}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${row.owner_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${row.owner_street}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${row.owner_city}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${row.owner_psc}</t>
   </si>
   <si>
     <t xml:space="preserve">${row.spoluvlastnicky_podiel}</t>
@@ -157,7 +181,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,11 +191,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF729FCF"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF77BC65"/>
+        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -179,6 +209,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -205,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,11 +271,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,6 +293,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -320,7 +369,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -339,13 +388,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.7"/>
@@ -356,15 +405,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="13.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="18.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="71.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="16.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="14" style="1" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="5" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="51.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="16.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="18" style="1" width="8.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -392,72 +441,91 @@
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="K2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K3" s="11"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="13"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="11"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="13"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated report template + finished corporate owner parsing
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/xlsx/garages_report.xlsx
+++ b/src/main/resources/templates/xlsx/garages_report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve">Obec</t>
   </si>
@@ -49,19 +49,22 @@
     <t xml:space="preserve">Iné údaje</t>
   </si>
   <si>
+    <t xml:space="preserve">Meno vlastníka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ulica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSČ</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dátum narodenia</t>
   </si>
   <si>
-    <t xml:space="preserve">Priezvisko a Meno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ulica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PSČ</t>
+    <t xml:space="preserve">IČO</t>
   </si>
   <si>
     <t xml:space="preserve">Spoluvlastnícky podiel</t>
@@ -97,19 +100,22 @@
     <t xml:space="preserve">${row.ine_udaje}</t>
   </si>
   <si>
+    <t xml:space="preserve">${row.owner_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${row.owner_street}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${row.owner_city}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${row.owner_postal_code}</t>
+  </si>
+  <si>
     <t xml:space="preserve">${row.owner_birthDate}</t>
   </si>
   <si>
-    <t xml:space="preserve">${row.owner_name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${row.owner_street}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${row.owner_city}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${row.owner_psc}</t>
+    <t xml:space="preserve">${row.owner_corporate_id}</t>
   </si>
   <si>
     <t xml:space="preserve">${row.spoluvlastnicky_podiel}</t>
@@ -388,10 +394,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -405,12 +413,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="13.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="18.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="24.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="5" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="16.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="18" style="1" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="5" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="5" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="51.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="33.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="19" style="1" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,76 +467,82 @@
       <c r="N1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="K2" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="L2" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="P2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="Q2" s="6" t="s">
         <v>33</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O3" s="14"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="16"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>